<commit_message>
Updated overview (thermal demand still in progress)
</commit_message>
<xml_diff>
--- a/docs/source/overview/OverviewFigures/tables.xlsx
+++ b/docs/source/overview/OverviewFigures/tables.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C70400E-7199-4894-A930-3A1F213979A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFC899A-B75F-4D06-94AB-7033B1404916}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="548" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="548" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Appliances" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="56">
   <si>
     <t>Constant Load</t>
   </si>
@@ -29,10 +29,6 @@
     <t>Time varying load</t>
   </si>
   <si>
-    <t>Fridge
-Freezer</t>
-  </si>
-  <si>
     <t>Fixed duration</t>
   </si>
   <si>
@@ -43,34 +39,191 @@
   </si>
   <si>
     <t>Stochastic duration</t>
+  </si>
+  <si>
+    <t>Washing machine
+Washer dryer</t>
+  </si>
+  <si>
+    <t>Chest freezer
+Fridge freezer
+Refrigerator
+Upright freezer
+Fridge
+Freezer
+Clock</t>
   </si>
   <si>
     <t>Iron 
 Telephone                                                                                                                                                                                                                                                                Computer                                                                                                                                                                                                                                                                Laptop 
 Tablet
 Printer
+Fax
 DVD &amp; Blue-ray
+VCR / DVD
+TV re
 Game console
 Hob
 Micro-wave
-Kattle</t>
-  </si>
-  <si>
-    <t>Washing machine
-Washer dryer</t>
-  </si>
-  <si>
-    <t>TV
+Kattle
+Answer machine
+Cassette/CD player
+Cordless telephone
+Hi-Fi
+TV
 Oven
+Small cooking (group)
 Dish washer
 Dryer</t>
+  </si>
+  <si>
+    <t>Chest freezer</t>
+  </si>
+  <si>
+    <t>Fridge freezer</t>
+  </si>
+  <si>
+    <t>Refrigerator</t>
+  </si>
+  <si>
+    <t>Upright freezer</t>
+  </si>
+  <si>
+    <t>Answer machine</t>
+  </si>
+  <si>
+    <t>Cassette / CD Player</t>
+  </si>
+  <si>
+    <t>Clock</t>
+  </si>
+  <si>
+    <t>Cordless telephone</t>
+  </si>
+  <si>
+    <t>Hi-Fi</t>
+  </si>
+  <si>
+    <t>Iron</t>
+  </si>
+  <si>
+    <t>Vacuum</t>
+  </si>
+  <si>
+    <t>Fax</t>
+  </si>
+  <si>
+    <t>Personal computer</t>
+  </si>
+  <si>
+    <t>Printer</t>
+  </si>
+  <si>
+    <t>VCR / DVD</t>
+  </si>
+  <si>
+    <t>TV Receiver box</t>
+  </si>
+  <si>
+    <t>Hob</t>
+  </si>
+  <si>
+    <t>Oven</t>
+  </si>
+  <si>
+    <t>Microwave</t>
+  </si>
+  <si>
+    <t>Kettle</t>
+  </si>
+  <si>
+    <t>Small cooking (group)</t>
+  </si>
+  <si>
+    <t>Dish washer</t>
+  </si>
+  <si>
+    <t>Tumble dryer</t>
+  </si>
+  <si>
+    <t>Washing machine</t>
+  </si>
+  <si>
+    <t>Washer dryer</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>Load profile</t>
+  </si>
+  <si>
+    <t>Usage duration</t>
+  </si>
+  <si>
+    <t>Usage Pattern</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Fridge</t>
+  </si>
+  <si>
+    <t>Freezer</t>
+  </si>
+  <si>
+    <t>constant</t>
+  </si>
+  <si>
+    <t>fixed</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>Telephone</t>
+  </si>
+  <si>
+    <t>Computer</t>
+  </si>
+  <si>
+    <t>Laptop</t>
+  </si>
+  <si>
+    <t>TV</t>
+  </si>
+  <si>
+    <t>Tablet</t>
+  </si>
+  <si>
+    <t>DVD / Blue-ray</t>
+  </si>
+  <si>
+    <t>Game console</t>
+  </si>
+  <si>
+    <t>activity</t>
+  </si>
+  <si>
+    <t>stochastic</t>
+  </si>
+  <si>
+    <t>time-varying</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    Characteristics
+Appliances</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +234,48 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri "/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -107,7 +302,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -227,11 +422,218 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalDown="1">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="medium">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -276,9 +678,76 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{DE206D80-66BD-48ED-9133-79F1CEEF12CA}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -558,11 +1027,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="9.06640625" style="1"/>
     <col min="2" max="2" width="13.06640625" style="1" customWidth="1"/>
@@ -571,8 +1040,8 @@
     <col min="6" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="5" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:7" ht="14.65" thickBot="1"/>
+    <row r="5" spans="2:7" ht="14.65" thickBot="1">
       <c r="D5" s="4" t="s">
         <v>0</v>
       </c>
@@ -580,52 +1049,50 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:7" ht="92.65" customHeight="1">
       <c r="B6" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>4</v>
-      </c>
       <c r="D6" s="6" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="2:7" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:7" ht="35" customHeight="1" thickBot="1">
       <c r="B7" s="15"/>
       <c r="C7" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" spans="2:7" ht="156.75" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:7">
       <c r="B8" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>7</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D8" s="13"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="2:7" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:7" ht="370.9" thickBot="1">
       <c r="B9" s="15"/>
       <c r="C9" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G9" s="8"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:7">
       <c r="E11" s="8"/>
     </row>
   </sheetData>
@@ -640,14 +1107,679 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C663398-67F9-47F6-9197-88C28BE312C9}">
-  <dimension ref="A1"/>
+  <dimension ref="C17:H52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="2" width="9.06640625" style="1"/>
+    <col min="3" max="3" width="17.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.59765625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="6.59765625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.06640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="17" spans="3:8" ht="14.65" thickBot="1"/>
+    <row r="18" spans="3:8" ht="27" thickBot="1">
+      <c r="C18" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8">
+      <c r="C19" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="H19" s="33"/>
+    </row>
+    <row r="20" spans="3:8">
+      <c r="C20" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="23"/>
+    </row>
+    <row r="21" spans="3:8">
+      <c r="C21" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H21" s="23"/>
+    </row>
+    <row r="22" spans="3:8">
+      <c r="C22" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" s="23"/>
+    </row>
+    <row r="23" spans="3:8">
+      <c r="C23" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23" s="22"/>
+      <c r="H23" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8">
+      <c r="C24" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24" s="22"/>
+      <c r="H24" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8">
+      <c r="C25" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H25" s="23"/>
+    </row>
+    <row r="26" spans="3:8">
+      <c r="C26" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H26" s="23"/>
+    </row>
+    <row r="27" spans="3:8">
+      <c r="C27" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G27" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H27" s="23"/>
+    </row>
+    <row r="28" spans="3:8">
+      <c r="C28" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H28" s="23"/>
+    </row>
+    <row r="29" spans="3:8">
+      <c r="C29" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29" s="22"/>
+      <c r="H29" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="3:8">
+      <c r="C30" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G30" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H30" s="23"/>
+    </row>
+    <row r="31" spans="3:8">
+      <c r="C31" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G31" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H31" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="3:8">
+      <c r="C32" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G32" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H32" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8">
+      <c r="C33" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G33" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H33" s="23"/>
+    </row>
+    <row r="34" spans="3:8">
+      <c r="C34" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G34" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H34" s="23"/>
+    </row>
+    <row r="35" spans="3:8">
+      <c r="C35" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G35" s="22"/>
+      <c r="H35" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8">
+      <c r="C36" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F36" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G36" s="22"/>
+      <c r="H36" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="3:8">
+      <c r="C37" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G37" s="22"/>
+      <c r="H37" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="3:8">
+      <c r="C38" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G38" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H38" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8">
+      <c r="C39" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G39" s="22"/>
+      <c r="H39" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="3:8">
+      <c r="C40" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E40" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G40" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H40" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="3:8">
+      <c r="C41" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E41" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F41" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G41" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H41" s="23"/>
+    </row>
+    <row r="42" spans="3:8">
+      <c r="C42" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F42" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G42" s="22"/>
+      <c r="H42" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="3:8">
+      <c r="C43" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F43" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G43" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H43" s="23"/>
+    </row>
+    <row r="44" spans="3:8">
+      <c r="C44" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E44" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F44" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H44" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="3:8">
+      <c r="C45" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F45" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G45" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H45" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="3:8">
+      <c r="C46" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E46" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F46" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G46" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H46" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="3:8">
+      <c r="C47" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D47" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E47" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F47" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G47" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H47" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="3:8">
+      <c r="C48" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D48" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F48" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G48" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H48" s="23"/>
+    </row>
+    <row r="49" spans="3:8">
+      <c r="C49" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E49" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F49" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G49" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H49" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="3:8">
+      <c r="C50" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F50" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G50" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H50" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="3:8">
+      <c r="C51" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D51" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F51" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G51" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H51" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8" ht="14.65" thickBot="1">
+      <c r="C52" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D52" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E52" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F52" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="G52" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="H52" s="25"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>